<commit_message>
[Esakkimuthu] Add Celery implementation for account opening email
</commit_message>
<xml_diff>
--- a/user_list.xlsx
+++ b/user_list.xlsx
@@ -462,21 +462,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>adam@gmail.com</t>
+          <t>bruce@gmail.com</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Adam</t>
+          <t>Bruce</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mettews</t>
+          <t>Wayne</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45128.7368401979</v>
+        <v>45131.5644113271</v>
       </c>
     </row>
     <row r="3">
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="D3" s="2" t="n">
-        <v>45128.74729519995</v>
+        <v>45131.60717907707</v>
       </c>
     </row>
     <row r="4">
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>45128.74729521712</v>
+        <v>45131.60718010938</v>
       </c>
     </row>
     <row r="5">
@@ -536,7 +536,7 @@
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>45128.74729522832</v>
+        <v>45131.60718113895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>